<commit_message>
updated from work on galactic search at summit
</commit_message>
<xml_diff>
--- a/characterization/ShooterTuning.xlsx
+++ b/characterization/ShooterTuning.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\bwg\rtools\droid2021\characterization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4335A849-7ACA-4849-8C8C-33EDCFE85E8F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E4D447BF-1274-46AF-8D9B-F9D68DB8192D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1422" yWindow="0" windowWidth="17280" windowHeight="8994" xr2:uid="{48843437-367F-4B93-9C44-6CCA3E74E663}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{48843437-367F-4B93-9C44-6CCA3E74E663}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -101,6 +102,1913 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-9.2804024496942971E-4"/>
+                  <c:y val="-3.9661708953047536E-4"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$3:$C$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>117</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$3:$D$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3700</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3815</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0E3B-4BAC-BFF7-04D64D7354A6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="101497343"/>
+        <c:axId val="101495679"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="101497343"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="101495679"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="101495679"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="101497343"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$6:$C$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>132</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>158</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>205</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>237</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$6:$D$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>7000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6350</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6050</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5700</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6560</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4ABA-4194-8643-08FD5D2C7344}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="97835919"/>
+        <c:axId val="97836335"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="97835919"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="97836335"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="97836335"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="97835919"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>59055</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>205740</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>59055</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DB0E4089-0FFE-4BF1-AF87-9CE3B6D0B6A5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>43815</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>89535</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>135255</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>89535</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C86671B6-EA0C-4B0E-AC26-9E1E7FB57092}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -403,7 +2311,7 @@
   <dimension ref="B2:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11:F15"/>
+      <selection activeCell="C6" sqref="C6:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -519,7 +2427,7 @@
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B10">
-        <f t="shared" ref="B10" si="1">C10-C9</f>
+        <f>C10-C9</f>
         <v>32</v>
       </c>
       <c r="C10">
@@ -531,5 +2439,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>